<commit_message>
Refactor - all references from complete genome isolates
</commit_message>
<xml_diff>
--- a/tabular/core/incomplete-genome-seqs.xlsx
+++ b/tabular/core/incomplete-genome-seqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/Flu-GLUE/tabular/core/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F908CBD-A5E7-7C46-898E-5114C277C50C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1346012C-909F-0D4F-8D78-AF3E87D388EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="680" windowWidth="17880" windowHeight="15480" xr2:uid="{6A54E187-03C7-444F-844F-19109E012297}"/>
   </bookViews>
@@ -725,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784DEF8A-681F-4E49-B5CD-BEC488A3242E}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D52" sqref="A1:D52"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A12" sqref="A1:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>